<commit_message>
test(data): Update test Excel file
- Replaced the content of `tests/files/excel file.xlsx` to reflect updated test cases or requirements.

This update ensures alignment with the latest test scenarios for data handling functionality.
</commit_message>
<xml_diff>
--- a/tests/files/excel file.xlsx
+++ b/tests/files/excel file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>NAME</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>FILE</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Glaiza Marie</t>
+  </si>
+  <si>
+    <t>glaiza.garay@powersource.group</t>
   </si>
 </sst>
 </file>
@@ -397,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,13 +476,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>